<commit_message>
Refactorizando el modelo de datos
Refactorizando el modelo de datos con cambios de nombre de tabla y agregando campos en EntidadSbbip

Modificando la tabla EntidadSbbip en su nombre y agregando nuevos campos en la misma arreglando unos
problema de informacion de contacto; además se actualizó y modificó los schemas.yml, el modelo de las clases
y el repositorio nuevo generado con el cambio de nombre de en la tabla EntidadSbbip y sus respectivas relaciones con las tablas ContraraB, ContraraSB y ContratarIp
</commit_message>
<xml_diff>
--- a/docs/backup/cuenta_2200555126.xlsx
+++ b/docs/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="329">
   <si>
     <t>D</t>
   </si>
@@ -1002,6 +1002,15 @@
   </si>
   <si>
     <t>36.73  </t>
+  </si>
+  <si>
+    <t>0005194711</t>
+  </si>
+  <si>
+    <t>300.00  </t>
+  </si>
+  <si>
+    <t>300.00</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1333,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -1339,52 +1348,52 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41793</v>
+        <v>41796</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>264</v>
+        <v>328</v>
       </c>
       <c r="H1" t="str">
         <f t="shared" ref="H1:H2" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-03'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0009269866', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 36.73  , 'mo_saldo' =&gt; 0.00, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-03 20:20:57'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-06'), 'mo_concepto' =&gt; 'DEPOSITO', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0005194711', 'mo_oficina' =&gt; 'EL GIRON', 'mo_monto' =&gt; 300.00  , 'mo_saldo' =&gt; 300.00, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-07 15:28:28'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41792</v>
+        <v>41793</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>323</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1392,114 +1401,114 @@
         <v>41792</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41788</v>
+        <v>41792</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>316</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>317</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41787</v>
+        <v>41788</v>
       </c>
       <c r="B5" t="s">
-        <v>302</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>304</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41786</v>
+        <v>41787</v>
       </c>
       <c r="B6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>304</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41785</v>
+        <v>41786</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>306</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>310</v>
+        <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1507,22 +1516,22 @@
         <v>41785</v>
       </c>
       <c r="B8" t="s">
-        <v>312</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1530,27 +1539,27 @@
         <v>41785</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>312</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41781</v>
+        <v>41785</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1559,108 +1568,108 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>260</v>
+        <v>297</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>6</v>
+        <v>298</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>261</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41779</v>
+        <v>41781</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>263</v>
+        <v>6</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41767</v>
+        <v>41779</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41766</v>
+        <v>41767</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41765</v>
+        <v>41766</v>
       </c>
       <c r="B14" t="s">
-        <v>271</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,22 +1677,22 @@
         <v>41765</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>271</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1697,62 +1706,62 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41764</v>
+        <v>41765</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41761</v>
+        <v>41764</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>281</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,19 +1772,19 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1786,10 +1795,10 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -1798,7 +1807,7 @@
         <v>289</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,16 +1821,16 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1832,70 +1841,70 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>67</v>
+        <v>294</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41759</v>
+        <v>41761</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>254</v>
+        <v>295</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>255</v>
+        <v>67</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>256</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41758</v>
+        <v>41759</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41757</v>
+        <v>41758</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -1904,16 +1913,16 @@
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1927,16 +1936,16 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1944,45 +1953,45 @@
         <v>41757</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E27" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41754</v>
+        <v>41757</v>
       </c>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>243</v>
+        <v>67</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1990,22 +1999,22 @@
         <v>41754</v>
       </c>
       <c r="B29" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2013,13 +2022,13 @@
         <v>41754</v>
       </c>
       <c r="B30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
@@ -2028,7 +2037,7 @@
         <v>247</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2036,68 +2045,68 @@
         <v>41754</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41752</v>
+        <v>41754</v>
       </c>
       <c r="B32" t="s">
-        <v>223</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41751</v>
+        <v>41752</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>223</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2105,91 +2114,91 @@
         <v>41751</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41750</v>
+        <v>41751</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>221</v>
+        <v>6</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41746</v>
+        <v>41750</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="E36" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41744</v>
+        <v>41746</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2197,22 +2206,22 @@
         <v>41744</v>
       </c>
       <c r="B38" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>203</v>
+        <v>67</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2220,22 +2229,22 @@
         <v>41744</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2249,39 +2258,39 @@
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2295,16 +2304,16 @@
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>214</v>
+        <v>6</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2312,45 +2321,45 @@
         <v>41743</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41740</v>
+        <v>41743</v>
       </c>
       <c r="B44" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2358,45 +2367,45 @@
         <v>41740</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41739</v>
+        <v>41740</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2404,91 +2413,91 @@
         <v>41739</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="C47" t="s">
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E47" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>67</v>
+        <v>191</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41738</v>
+        <v>41739</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="E48" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>165</v>
+        <v>67</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41737</v>
+        <v>41738</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41736</v>
+        <v>41737</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E50" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>174</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2496,22 +2505,22 @@
         <v>41736</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E51" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2519,45 +2528,45 @@
         <v>41736</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41731</v>
+        <v>41736</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E53" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2565,45 +2574,45 @@
         <v>41731</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41729</v>
+        <v>41731</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2611,27 +2620,27 @@
         <v>41729</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>41725</v>
+        <v>41729</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
@@ -2640,16 +2649,16 @@
         <v>4</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2657,45 +2666,45 @@
         <v>41725</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E59" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2703,22 +2712,22 @@
         <v>41722</v>
       </c>
       <c r="B60" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E60" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2726,22 +2735,22 @@
         <v>41722</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E61" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2749,128 +2758,128 @@
         <v>41722</v>
       </c>
       <c r="B62" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E62" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41719</v>
+        <v>41722</v>
       </c>
       <c r="B63" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E63" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>41712</v>
+        <v>41719</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E64" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>41708</v>
+        <v>41712</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E65" t="s">
         <v>5</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>41705</v>
+        <v>41708</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E66" t="s">
         <v>5</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E67" t="s">
         <v>5</v>
@@ -2879,7 +2888,7 @@
         <v>133</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2887,22 +2896,22 @@
         <v>41703</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E68" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2910,68 +2919,68 @@
         <v>41703</v>
       </c>
       <c r="B69" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E69" t="s">
         <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E70" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E71" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2985,7 +2994,7 @@
         <v>4</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
@@ -2994,30 +3003,30 @@
         <v>67</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B73" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E73" t="s">
         <v>5</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3028,10 +3037,10 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E74" t="s">
         <v>5</v>
@@ -3040,53 +3049,53 @@
         <v>114</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E75" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C76" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3094,45 +3103,45 @@
         <v>41680</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C77" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E77" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B78" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3140,36 +3149,36 @@
         <v>41677</v>
       </c>
       <c r="B79" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C79" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E79" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C80" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E80" t="s">
         <v>5</v>
@@ -3178,76 +3187,76 @@
         <v>101</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>41674</v>
+        <v>41676</v>
       </c>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E81" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C82" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E82" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B83" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E83" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3255,22 +3264,22 @@
         <v>41666</v>
       </c>
       <c r="B84" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84" t="s">
         <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E84" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3278,22 +3287,22 @@
         <v>41666</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C85" t="s">
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E85" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3301,45 +3310,45 @@
         <v>41666</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C86" t="s">
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E86" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C87" t="s">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E87" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3347,22 +3356,22 @@
         <v>41660</v>
       </c>
       <c r="B88" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3370,68 +3379,68 @@
         <v>41660</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C89" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E89" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B90" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E90" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B91" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C91" t="s">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E91" t="s">
         <v>1</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3439,50 +3448,50 @@
         <v>41655</v>
       </c>
       <c r="B92" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E92" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C93" t="s">
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B94" t="s">
         <v>3</v>
@@ -3491,39 +3500,39 @@
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E94" t="s">
         <v>5</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B95" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C95" t="s">
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E95" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3531,68 +3540,68 @@
         <v>41648</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B97" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C97" t="s">
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E97" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B98" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C98" t="s">
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E98" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3600,22 +3609,22 @@
         <v>41646</v>
       </c>
       <c r="B99" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C99" t="s">
         <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E99" t="s">
         <v>12</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3623,22 +3632,22 @@
         <v>41646</v>
       </c>
       <c r="B100" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C100" t="s">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E100" t="s">
         <v>12</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3646,101 +3655,118 @@
         <v>41646</v>
       </c>
       <c r="B101" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C101" t="s">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E101" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B102" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C102" t="s">
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E102" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>41642</v>
+        <v>41645</v>
       </c>
       <c r="B103" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C103" t="s">
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E103" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B104" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E104" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>41641</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>68</v>
       </c>
-      <c r="C104" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="2" t="s">
+      <c r="C105" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E105" t="s">
         <v>1</v>
       </c>
-      <c r="F104" s="3" t="s">
+      <c r="F105" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G104" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
-      <c r="D106"/>
-      <c r="F106"/>
-      <c r="G106"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
@@ -3760,6 +3786,12 @@
       <c r="F109"/>
       <c r="G109"/>
     </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="D110"/>
+      <c r="F110"/>
+      <c r="G110"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizando estilos bootstrap v3.2.0
Actualizando estilos del sitio web con la herramienta libre bootstrap v3.2.0

Bootstrap v3.2.0 saca una nueva version y se la aplica rapidamente.
</commit_message>
<xml_diff>
--- a/docs/backup/cuenta_2200555126.xlsx
+++ b/docs/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="475">
   <si>
     <t>D</t>
   </si>
@@ -1443,6 +1443,12 @@
   </si>
   <si>
     <t>188.29</t>
+  </si>
+  <si>
+    <t>0010920736</t>
+  </si>
+  <si>
+    <t>2.83</t>
   </si>
 </sst>
 </file>
@@ -1765,10 +1771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H1:H8"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,26 +1789,26 @@
         <v>41848</v>
       </c>
       <c r="B1" t="s">
-        <v>449</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>450</v>
+        <v>473</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>370</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H8" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-28'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/AKI MOLINEROS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002949333', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 5.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H9" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-28'), 'mo_concepto' =&gt; '2200555126/0995935959', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0010920736', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 3.00  , 'mo_saldo' =&gt; 2.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-28 20:18:3'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1810,80 +1816,68 @@
         <v>41848</v>
       </c>
       <c r="B2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>454</v>
+        <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-28'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA (MALL EL JARDIN', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002748157', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 3.94  , 'mo_saldo' =&gt; 25.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41844</v>
+        <v>41848</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>452</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-24'), 'mo_concepto' =&gt; 'DEPOSITO', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0004801502', 'mo_oficina' =&gt; 'EL GIRON', 'mo_monto' =&gt; 18.67  , 'mo_saldo' =&gt; 29.77, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41842</v>
+        <v>41844</v>
       </c>
       <c r="B4" t="s">
-        <v>459</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-22'), 'mo_concepto' =&gt; 'RETIRO ATM BP N/EL GIRON-5', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004586361', 'mo_oficina' =&gt; 'EL GIRON', 'mo_monto' =&gt; 10.00  , 'mo_saldo' =&gt; 11.10, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1891,26 +1885,22 @@
         <v>41842</v>
       </c>
       <c r="B5" t="s">
-        <v>368</v>
+        <v>459</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>370</v>
+        <v>461</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-22'), 'mo_concepto' =&gt; '2200555126/0998453098', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002358390', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 3.00  , 'mo_saldo' =&gt; 21.10, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,26 +1908,22 @@
         <v>41842</v>
       </c>
       <c r="B6" t="s">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>97</v>
+        <v>370</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-22'), 'mo_concepto' =&gt; 'CONSUMO VISA NA ESTACION DE SERVICIO A', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000846283', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 15.26  , 'mo_saldo' =&gt; 24.10, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1945,53 +1931,45 @@
         <v>41842</v>
       </c>
       <c r="B7" t="s">
-        <v>467</v>
+        <v>400</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>469</v>
+        <v>97</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-22'), 'mo_concepto' =&gt; '14199571-MASTERCARD-RA-518114000072', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000568133', 'mo_oficina' =&gt; 'SERVICIOS CENTRALES', 'mo_monto' =&gt; 148.93  , 'mo_saldo' =&gt; 39.36, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41841</v>
+        <v>41842</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>467</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>9</v>
+        <v>469</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-21'), 'mo_concepto' =&gt; 'RETIRO ATM BP N/GIRON 2', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0011019252', 'mo_oficina' =&gt; 'EL GIRON', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 188.29, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-27 16:49:48'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1999,91 +1977,91 @@
         <v>41841</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>439</v>
+        <v>471</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>440</v>
+        <v>9</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>441</v>
+        <v>472</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41837</v>
+        <v>41841</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E10" t="s">
-        <v>444</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>440</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41836</v>
+        <v>41837</v>
       </c>
       <c r="B11" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E11" t="s">
-        <v>331</v>
+        <v>444</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41835</v>
+        <v>41836</v>
       </c>
       <c r="B12" t="s">
-        <v>374</v>
+        <v>446</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>375</v>
+        <v>447</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>331</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>376</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2091,22 +2069,22 @@
         <v>41835</v>
       </c>
       <c r="B13" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2114,22 +2092,22 @@
         <v>41835</v>
       </c>
       <c r="B14" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>382</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2137,22 +2115,22 @@
         <v>41835</v>
       </c>
       <c r="B15" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>67</v>
+        <v>382</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2160,22 +2138,22 @@
         <v>41835</v>
       </c>
       <c r="B16" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>389</v>
+        <v>67</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2183,22 +2161,22 @@
         <v>41835</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>387</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>327</v>
+        <v>389</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2206,22 +2184,22 @@
         <v>41835</v>
       </c>
       <c r="B18" t="s">
-        <v>368</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2229,68 +2207,68 @@
         <v>41835</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>368</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>141</v>
+        <v>370</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41834</v>
+        <v>41835</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>398</v>
+        <v>141</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41830</v>
+        <v>41834</v>
       </c>
       <c r="B21" t="s">
-        <v>400</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>97</v>
+        <v>398</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,45 +2276,45 @@
         <v>41830</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>400</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>404</v>
+        <v>97</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41829</v>
+        <v>41830</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>438</v>
+        <v>404</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>264</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,13 +2322,13 @@
         <v>41829</v>
       </c>
       <c r="B24" t="s">
-        <v>407</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -2359,30 +2337,30 @@
         <v>438</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>437</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41827</v>
+        <v>41829</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>407</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>410</v>
+        <v>438</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>264</v>
+        <v>437</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2390,13 +2368,13 @@
         <v>41827</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -2405,7 +2383,7 @@
         <v>410</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>412</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2413,22 +2391,22 @@
         <v>41827</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>264</v>
+        <v>412</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2436,22 +2414,22 @@
         <v>41827</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>417</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2465,16 +2443,16 @@
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,22 +2460,22 @@
         <v>41827</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>27</v>
+        <v>419</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2511,39 +2489,39 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>424</v>
+        <v>27</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41824</v>
+        <v>41827</v>
       </c>
       <c r="B32" t="s">
-        <v>426</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E32" t="s">
-        <v>428</v>
+        <v>5</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2551,7 +2529,7 @@
         <v>41824</v>
       </c>
       <c r="B33" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -2563,10 +2541,10 @@
         <v>428</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2574,22 +2552,22 @@
         <v>41824</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>431</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>428</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>266</v>
+        <v>432</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2597,137 +2575,137 @@
         <v>41824</v>
       </c>
       <c r="B35" t="s">
-        <v>144</v>
+        <v>306</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E35" t="s">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>9</v>
+        <v>266</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41823</v>
+        <v>41824</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>348</v>
+        <v>436</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>349</v>
+        <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>350</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41821</v>
+        <v>41823</v>
       </c>
       <c r="B37" t="s">
-        <v>351</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E37" t="s">
-        <v>331</v>
+        <v>5</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>67</v>
+        <v>349</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41820</v>
+        <v>41821</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>351</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E38" t="s">
-        <v>19</v>
+        <v>331</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>355</v>
+        <v>67</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41817</v>
+        <v>41820</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E39" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>67</v>
+        <v>355</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41816</v>
+        <v>41817</v>
       </c>
       <c r="B40" t="s">
-        <v>306</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>264</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,45 +2713,45 @@
         <v>41816</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>306</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>266</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>361</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41813</v>
+        <v>41816</v>
       </c>
       <c r="B42" t="s">
-        <v>362</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>364</v>
+        <v>266</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>264</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2781,91 +2759,91 @@
         <v>41813</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>362</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>367</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41810</v>
+        <v>41813</v>
       </c>
       <c r="B44" t="s">
-        <v>368</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E44" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41809</v>
+        <v>41810</v>
       </c>
       <c r="B45" t="s">
-        <v>306</v>
+        <v>368</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>67</v>
+        <v>370</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41807</v>
+        <v>41809</v>
       </c>
       <c r="B46" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>330</v>
+        <v>372</v>
       </c>
       <c r="E46" t="s">
-        <v>331</v>
+        <v>8</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>332</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,45 +2851,45 @@
         <v>41807</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>329</v>
       </c>
       <c r="C47" t="s">
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41806</v>
+        <v>41807</v>
       </c>
       <c r="B48" t="s">
-        <v>306</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2919,160 +2897,160 @@
         <v>41806</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>306</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>338</v>
+        <v>9</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41803</v>
+        <v>41806</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>286</v>
+        <v>338</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41802</v>
+        <v>41803</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>343</v>
+        <v>286</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41799</v>
+        <v>41802</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E52" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41796</v>
+        <v>41799</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>326</v>
+        <v>345</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>327</v>
+        <v>346</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>41793</v>
+        <v>41796</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E54" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>264</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41792</v>
+        <v>41793</v>
       </c>
       <c r="B55" t="s">
-        <v>320</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E55" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>323</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3080,114 +3058,114 @@
         <v>41792</v>
       </c>
       <c r="B56" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>41788</v>
+        <v>41792</v>
       </c>
       <c r="B57" t="s">
-        <v>197</v>
+        <v>316</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="E57" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>9</v>
+        <v>317</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>41787</v>
+        <v>41788</v>
       </c>
       <c r="B58" t="s">
-        <v>302</v>
+        <v>197</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E58" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>304</v>
+        <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>41786</v>
+        <v>41787</v>
       </c>
       <c r="B59" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>9</v>
+        <v>304</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>41785</v>
+        <v>41786</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>306</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E60" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>310</v>
+        <v>9</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3195,22 +3173,22 @@
         <v>41785</v>
       </c>
       <c r="B61" t="s">
-        <v>312</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E61" t="s">
         <v>1</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3218,27 +3196,27 @@
         <v>41785</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>312</v>
       </c>
       <c r="C62" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41781</v>
+        <v>41785</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
@@ -3247,108 +3225,108 @@
         <v>4</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>260</v>
+        <v>297</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>6</v>
+        <v>298</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>261</v>
+        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>41779</v>
+        <v>41781</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E64" t="s">
         <v>5</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>263</v>
+        <v>6</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>41767</v>
+        <v>41779</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E65" t="s">
         <v>5</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>41766</v>
+        <v>41767</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E66" t="s">
         <v>5</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41765</v>
+        <v>41766</v>
       </c>
       <c r="B67" t="s">
-        <v>271</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E67" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3356,22 +3334,22 @@
         <v>41765</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>271</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E68" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3385,62 +3363,62 @@
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E69" t="s">
         <v>5</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>41764</v>
+        <v>41765</v>
       </c>
       <c r="B70" t="s">
-        <v>281</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E70" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>41761</v>
+        <v>41764</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>281</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E71" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3451,19 +3429,19 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3474,10 +3452,10 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E73" t="s">
         <v>5</v>
@@ -3486,7 +3464,7 @@
         <v>289</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3500,16 +3478,16 @@
         <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E74" t="s">
         <v>5</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3520,70 +3498,70 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E75" t="s">
         <v>5</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>67</v>
+        <v>294</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>41759</v>
+        <v>41761</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>254</v>
+        <v>295</v>
       </c>
       <c r="E76" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>255</v>
+        <v>67</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>256</v>
+        <v>296</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>41758</v>
+        <v>41759</v>
       </c>
       <c r="B77" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E77" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>41757</v>
+        <v>41758</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -3592,16 +3570,16 @@
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="E78" t="s">
         <v>1</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3615,16 +3593,16 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E79" t="s">
         <v>1</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3632,45 +3610,45 @@
         <v>41757</v>
       </c>
       <c r="B80" t="s">
-        <v>238</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E80" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>41754</v>
+        <v>41757</v>
       </c>
       <c r="B81" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C81" t="s">
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E81" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>243</v>
+        <v>67</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3678,22 +3656,22 @@
         <v>41754</v>
       </c>
       <c r="B82" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C82" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E82" t="s">
         <v>1</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3701,13 +3679,13 @@
         <v>41754</v>
       </c>
       <c r="B83" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E83" t="s">
         <v>1</v>
@@ -3716,7 +3694,7 @@
         <v>247</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3724,68 +3702,68 @@
         <v>41754</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>248</v>
       </c>
       <c r="C84" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>41752</v>
+        <v>41754</v>
       </c>
       <c r="B85" t="s">
-        <v>223</v>
+        <v>32</v>
       </c>
       <c r="C85" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="E85" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>41751</v>
+        <v>41752</v>
       </c>
       <c r="B86" t="s">
-        <v>2</v>
+        <v>223</v>
       </c>
       <c r="C86" t="s">
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E86" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3793,91 +3771,91 @@
         <v>41751</v>
       </c>
       <c r="B87" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E87" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>41750</v>
+        <v>41751</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
+        <v>144</v>
       </c>
       <c r="C88" t="s">
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="E88" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>221</v>
+        <v>6</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>41746</v>
+        <v>41750</v>
       </c>
       <c r="B89" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C89" t="s">
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="E89" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>41744</v>
+        <v>41746</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="C90" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E90" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3885,22 +3863,22 @@
         <v>41744</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C91" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E91" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>203</v>
+        <v>67</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3908,22 +3886,22 @@
         <v>41744</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E92" t="s">
         <v>1</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3937,39 +3915,39 @@
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E93" t="s">
         <v>1</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B94" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C94" t="s">
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E94" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3983,16 +3961,16 @@
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E95" t="s">
         <v>5</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>214</v>
+        <v>6</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4000,45 +3978,45 @@
         <v>41743</v>
       </c>
       <c r="B96" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E96" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>41740</v>
+        <v>41743</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="E97" t="s">
         <v>1</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4046,45 +4024,45 @@
         <v>41740</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="C98" t="s">
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E98" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>41739</v>
+        <v>41740</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>42</v>
       </c>
       <c r="C99" t="s">
         <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E99" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,91 +4070,91 @@
         <v>41739</v>
       </c>
       <c r="B100" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="C100" t="s">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E100" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>67</v>
+        <v>191</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>41738</v>
+        <v>41739</v>
       </c>
       <c r="B101" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C101" t="s">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="E101" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>165</v>
+        <v>67</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>41737</v>
+        <v>41738</v>
       </c>
       <c r="B102" t="s">
         <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E102" t="s">
         <v>5</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>41736</v>
+        <v>41737</v>
       </c>
       <c r="B103" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E103" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>174</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4184,22 +4162,22 @@
         <v>41736</v>
       </c>
       <c r="B104" t="s">
-        <v>59</v>
+        <v>175</v>
       </c>
       <c r="C104" t="s">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E104" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4207,45 +4185,45 @@
         <v>41736</v>
       </c>
       <c r="B105" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C105" t="s">
         <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E105" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>41731</v>
+        <v>41736</v>
       </c>
       <c r="B106" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C106" t="s">
         <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E106" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4253,45 +4231,45 @@
         <v>41731</v>
       </c>
       <c r="B107" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E107" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>41729</v>
+        <v>41731</v>
       </c>
       <c r="B108" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C108" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E108" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4299,27 +4277,27 @@
         <v>41729</v>
       </c>
       <c r="B109" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E109" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>41725</v>
+        <v>41729</v>
       </c>
       <c r="B110" t="s">
         <v>3</v>
@@ -4328,16 +4306,16 @@
         <v>4</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E110" t="s">
         <v>5</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4345,45 +4323,45 @@
         <v>41725</v>
       </c>
       <c r="B111" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E111" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B112" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C112" t="s">
         <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E112" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4391,22 +4369,22 @@
         <v>41722</v>
       </c>
       <c r="B113" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C113" t="s">
         <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E113" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4414,22 +4392,22 @@
         <v>41722</v>
       </c>
       <c r="B114" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C114" t="s">
         <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E114" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4437,128 +4415,128 @@
         <v>41722</v>
       </c>
       <c r="B115" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C115" t="s">
         <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E115" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>41719</v>
+        <v>41722</v>
       </c>
       <c r="B116" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C116" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E116" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>41712</v>
+        <v>41719</v>
       </c>
       <c r="B117" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="C117" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E117" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>41708</v>
+        <v>41712</v>
       </c>
       <c r="B118" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C118" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E118" t="s">
         <v>5</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>41705</v>
+        <v>41708</v>
       </c>
       <c r="B119" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C119" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E119" t="s">
         <v>5</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C120" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E120" t="s">
         <v>5</v>
@@ -4567,7 +4545,7 @@
         <v>133</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4575,22 +4553,22 @@
         <v>41703</v>
       </c>
       <c r="B121" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E121" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4598,68 +4576,68 @@
         <v>41703</v>
       </c>
       <c r="B122" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E122" t="s">
         <v>1</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B123" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E123" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C124" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E124" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4673,7 +4651,7 @@
         <v>4</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E125" t="s">
         <v>5</v>
@@ -4682,30 +4660,30 @@
         <v>67</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B126" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C126" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E126" t="s">
         <v>5</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4716,10 +4694,10 @@
         <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E127" t="s">
         <v>5</v>
@@ -4728,53 +4706,53 @@
         <v>114</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B128" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E128" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B129" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C129" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E129" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4782,45 +4760,45 @@
         <v>41680</v>
       </c>
       <c r="B130" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C130" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E130" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B131" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C131" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E131" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4828,36 +4806,36 @@
         <v>41677</v>
       </c>
       <c r="B132" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C132" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E132" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B133" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C133" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E133" t="s">
         <v>5</v>
@@ -4866,76 +4844,76 @@
         <v>101</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>41674</v>
+        <v>41676</v>
       </c>
       <c r="B134" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E134" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B135" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C135" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E135" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B136" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C136" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E136" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4943,22 +4921,22 @@
         <v>41666</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C137" t="s">
         <v>0</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E137" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4966,22 +4944,22 @@
         <v>41666</v>
       </c>
       <c r="B138" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C138" t="s">
         <v>0</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E138" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4989,45 +4967,45 @@
         <v>41666</v>
       </c>
       <c r="B139" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C139" t="s">
         <v>0</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E139" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C140" t="s">
         <v>0</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E140" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -5035,22 +5013,22 @@
         <v>41660</v>
       </c>
       <c r="B141" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C141" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E141" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -5058,68 +5036,68 @@
         <v>41660</v>
       </c>
       <c r="B142" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C142" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E142" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B143" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C143" t="s">
         <v>0</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E143" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B144" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C144" t="s">
         <v>0</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E144" t="s">
         <v>1</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -5127,50 +5105,50 @@
         <v>41655</v>
       </c>
       <c r="B145" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C145" t="s">
         <v>0</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E145" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C146" t="s">
         <v>0</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E146" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B147" t="s">
         <v>3</v>
@@ -5179,39 +5157,39 @@
         <v>0</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E147" t="s">
         <v>5</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B148" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C148" t="s">
         <v>0</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E148" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -5219,68 +5197,68 @@
         <v>41648</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C149" t="s">
         <v>0</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E149" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B150" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C150" t="s">
         <v>0</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E150" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B151" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C151" t="s">
         <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E151" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -5288,22 +5266,22 @@
         <v>41646</v>
       </c>
       <c r="B152" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C152" t="s">
         <v>0</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E152" t="s">
         <v>12</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5311,22 +5289,22 @@
         <v>41646</v>
       </c>
       <c r="B153" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C153" t="s">
         <v>0</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E153" t="s">
         <v>12</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -5334,101 +5312,118 @@
         <v>41646</v>
       </c>
       <c r="B154" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C154" t="s">
         <v>0</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E154" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B155" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C155" t="s">
         <v>0</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E155" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>41642</v>
+        <v>41645</v>
       </c>
       <c r="B156" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C156" t="s">
         <v>0</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E156" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B157" t="s">
+        <v>65</v>
+      </c>
+      <c r="C157" t="s">
+        <v>0</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E157" t="s">
+        <v>10</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
         <v>41641</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B158" t="s">
         <v>68</v>
       </c>
-      <c r="C157" t="s">
-        <v>0</v>
-      </c>
-      <c r="D157" s="2" t="s">
+      <c r="C158" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E158" t="s">
         <v>1</v>
       </c>
-      <c r="F157" s="3" t="s">
+      <c r="F158" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G157" s="3" t="s">
+      <c r="G158" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
-      <c r="D159"/>
-      <c r="F159"/>
-      <c r="G159"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
@@ -5448,6 +5443,12 @@
       <c r="F162"/>
       <c r="G162"/>
     </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+      <c r="D163"/>
+      <c r="F163"/>
+      <c r="G163"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>